<commit_message>
added more optimize tests
</commit_message>
<xml_diff>
--- a/data/tests/optimization_expected_results.xlsx
+++ b/data/tests/optimization_expected_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James H\git\CacheSimulator\data\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92D4094-1C6F-498A-BFB9-EF5096F7F15F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E763151-DCFE-410A-B453-A06A73FF9D3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{FAE95238-2509-45C5-A8DE-1B3CC67DCAF7}"/>
+    <workbookView xWindow="13680" yWindow="6084" windowWidth="17280" windowHeight="8964" xr2:uid="{FAE95238-2509-45C5-A8DE-1B3CC67DCAF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="50">
   <si>
     <t>Example</t>
   </si>
@@ -335,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -375,6 +375,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -921,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23663A99-338B-4259-AD48-C90E84F9C805}">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1695,457 +1699,627 @@
         <v>36</v>
       </c>
     </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="23">
+        <v>18</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>1</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="9">
+        <v>1</v>
+      </c>
+    </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="K16" t="s">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="23">
+        <v>25</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>0</v>
+      </c>
+      <c r="R16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
         <v>20</v>
       </c>
-      <c r="L16">
-        <f>SUM(L3:L14)</f>
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <f>SUM(M3:M14)</f>
-        <v>6</v>
-      </c>
-      <c r="N16">
-        <f>SUM(N3:N14)</f>
+      <c r="L19">
+        <f>SUM(L3:L16)</f>
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <f>SUM(M3:M16)</f>
+        <v>8</v>
+      </c>
+      <c r="N19">
+        <f>SUM(N3:N16)</f>
         <v>5</v>
       </c>
-      <c r="O16">
-        <f>SUM(L16:N16)</f>
-        <v>12</v>
-      </c>
-      <c r="P16">
-        <f>SUM(P3:P14)</f>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f>SUM(Q3:Q14)</f>
+      <c r="O19">
+        <f>SUM(L19:N19)</f>
+        <v>14</v>
+      </c>
+      <c r="P19">
+        <f>SUM(P3:P16)</f>
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <f>SUM(Q3:Q16)</f>
         <v>2</v>
       </c>
-      <c r="R16">
-        <f>SUM(R3:R14)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="R19">
+        <f>SUM(R3:R16)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B21" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E21" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F21" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G21" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="20"/>
-      <c r="I18" t="s">
+      <c r="H21" s="20"/>
+      <c r="I21" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="21" t="s">
+      <c r="J21" s="11"/>
+      <c r="K21" s="21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
         <f>G3</f>
         <v>29</v>
       </c>
-      <c r="B19">
+      <c r="B22">
         <f>L3</f>
         <v>0</v>
       </c>
-      <c r="C19">
+      <c r="C22">
         <f>M3</f>
         <v>0</v>
       </c>
-      <c r="D19">
+      <c r="D22">
         <f>N3</f>
         <v>1</v>
       </c>
-      <c r="E19">
-        <f>(IF(B19,A19,0))</f>
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <f>IF(C19,A19,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <f>IF(D19,A19,0)</f>
-        <v>29</v>
-      </c>
-      <c r="I19">
-        <f>SUM(A19:A30)/COUNT(A19:A30)</f>
-        <v>23.25</v>
-      </c>
-      <c r="K19">
-        <f>SUM(A19:A30)</f>
-        <v>279</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
-        <f t="shared" ref="A20:A30" si="0">G4</f>
+      <c r="E22">
+        <f>(IF(B22,A22,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>IF(C22,A22,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>IF(D22,A22,0)</f>
+        <v>29</v>
+      </c>
+      <c r="I22">
+        <f>SUM(A22:A35)/COUNT(A22:A35)</f>
+        <v>23</v>
+      </c>
+      <c r="K22">
+        <f>SUM(A22:A35)</f>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <f>G4</f>
         <v>2</v>
       </c>
-      <c r="B20">
-        <f t="shared" ref="B20:D20" si="1">L4</f>
-        <v>1</v>
-      </c>
-      <c r="C20">
+      <c r="B23">
+        <f>L4</f>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f>M4</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>N4</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:E33" si="0">(IF(B23,A23,0))</f>
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ref="F23:F33" si="1">IF(C23,A23,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G33" si="2">IF(D23,A23,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <f>G5</f>
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <f>L5</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>M5</f>
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f>N5</f>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <f>G6</f>
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <f>L6</f>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>M6</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>N6</f>
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E20">
-        <f t="shared" ref="E20:E30" si="2">(IF(B20,A20,0))</f>
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <f t="shared" ref="F20:F30" si="3">IF(C20,A20,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <f t="shared" ref="G20:G30" si="4">IF(D20,A20,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <f>G7</f>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f>L7</f>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f>M7</f>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f>N7</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <f>G8</f>
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <f>L8</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>M8</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f>N8</f>
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <f>G9</f>
         <v>19</v>
       </c>
-      <c r="B21">
-        <f t="shared" ref="B21:D21" si="5">L5</f>
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E21">
+      <c r="B28">
+        <f>L9</f>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>M9</f>
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f>N9</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <f>G10</f>
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <f>L10</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f>M10</f>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f>N10</f>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
+        <f>G11</f>
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f>L11</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f>M11</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f>N11</f>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
+        <f>G12</f>
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <f>L12</f>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>M12</f>
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f>N12</f>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="10">
+        <f>G13</f>
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <f>L13</f>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f>M13</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f>N13</f>
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="16">
+        <f>G14</f>
         <v>19</v>
       </c>
-      <c r="G21">
+      <c r="B33">
+        <f>L14</f>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f>M14</f>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f>N14</f>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
+        <f t="shared" ref="A34:A35" si="3">G15</f>
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ref="B34:D34" si="4">L15</f>
+        <v>0</v>
+      </c>
+      <c r="C34">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B22">
-        <f t="shared" ref="B22:D22" si="6">L6</f>
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="D34">
         <f t="shared" si="4"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <f t="shared" ref="B23:D23" si="7">L7</f>
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E35" si="5">(IF(B34,A34,0))</f>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F35" si="6">IF(C34,A34,0)</f>
+        <v>18</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ref="G34:G35" si="7">IF(D34,A34,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B24">
-        <f t="shared" ref="B24:D24" si="8">L8</f>
-        <v>0</v>
-      </c>
-      <c r="C24">
+      <c r="B35">
+        <f t="shared" ref="B35:D35" si="8">L16</f>
+        <v>0</v>
+      </c>
+      <c r="C35">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="D35">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="4"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B25">
-        <f t="shared" ref="B25:D25" si="9">L9</f>
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="B26">
-        <f t="shared" ref="B26:D26" si="10">L10</f>
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B27">
-        <f t="shared" ref="B27:D27" si="11">L11</f>
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="4"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="10">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B28">
-        <f t="shared" ref="B28:D28" si="12">L12</f>
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="10">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <f t="shared" ref="B29:D29" si="13">L13</f>
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="4"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="16">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B30">
-        <f t="shared" ref="B30:D30" si="14">L14</f>
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11" t="s">
+      <c r="G35">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D37" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="11">
-        <f>SUM(E19:E30)/COUNTIF(B19:B30,1)</f>
+      <c r="E37" s="11">
+        <f>SUM(E22:E35)/COUNTIF(B22:B35,1)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="11">
-        <f>SUM(F19:F30)/COUNTIF(C19:C30,1)</f>
-        <v>22</v>
-      </c>
-      <c r="G32" s="11">
-        <f>SUM(G19:G30)/COUNTIF(D19:D30,1)</f>
+      <c r="F37" s="11">
+        <f>SUM(F22:F35)/COUNTIF(C22:C35,1)</f>
+        <v>21.875</v>
+      </c>
+      <c r="G37" s="11">
+        <f>SUM(G22:G35)/COUNTIF(D22:D35,1)</f>
         <v>29</v>
       </c>
     </row>

</xml_diff>